<commit_message>
misc | map status update
</commit_message>
<xml_diff>
--- a/maps status.xlsx
+++ b/maps status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frtst\Documents\GitHub\Sauerract\Tesseract---Sauerbraten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E569C39-A578-4D7B-96B3-F2A39478FD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F11FED-C73F-4F61-8F9D-E90673B6D976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="255">
   <si>
     <t xml:space="preserve">aastha </t>
   </si>
@@ -795,6 +796,12 @@
   </si>
   <si>
     <t>oasis</t>
+  </si>
+  <si>
+    <t>skycastle-r</t>
+  </si>
+  <si>
+    <t>fc5</t>
   </si>
 </sst>
 </file>
@@ -1156,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2826,6 +2833,12 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>253</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="D110" t="s">
         <v>245</v>
       </c>
@@ -2834,6 +2847,12 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>254</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="D111" t="s">
         <v>247</v>
       </c>
@@ -2894,8 +2913,8 @@
         <v>126</v>
       </c>
       <c r="B124" s="5">
-        <f>COUNTA(B2:B109)</f>
-        <v>108</v>
+        <f>COUNTA(B2:B111)</f>
+        <v>110</v>
       </c>
       <c r="C124" s="5"/>
       <c r="D124" s="5" t="s">
@@ -2912,8 +2931,8 @@
         <v>125</v>
       </c>
       <c r="B125" s="5">
-        <f>COUNTIF(B2:B109, "Playable") + COUNTIF(B2:B109, "Optimized") + COUNTIF(B2:B109, "Remastered")</f>
-        <v>92</v>
+        <f>COUNTIF(B2:B111, "Playable") + COUNTIF(B2:B109, "Optimized") + COUNTIF(B2:B109, "Remastered")</f>
+        <v>94</v>
       </c>
       <c r="C125" s="5"/>
       <c r="D125" s="5" t="s">
@@ -2931,7 +2950,7 @@
       </c>
       <c r="B126" s="5">
         <f>(100/B124)*B125</f>
-        <v>85.18518518518519</v>
+        <v>85.454545454545453</v>
       </c>
       <c r="C126" s="5" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
fix | glitching maps
</commit_message>
<xml_diff>
--- a/maps status.xlsx
+++ b/maps status.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="254">
   <si>
     <t xml:space="preserve">CTF map name</t>
   </si>
@@ -791,7 +791,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -821,12 +821,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -900,31 +894,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1179,1791 +1173,1785 @@
   </sheetPr>
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C102" activeCellId="0" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="39.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="39.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="39.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="E9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="B11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="B12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="B15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="B16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="B17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="B18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="3" t="s">
+      <c r="E19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="B21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="B22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="B23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="B24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="B25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="B26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="3" t="s">
+      <c r="B27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="B28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="B29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="3" t="s">
+      <c r="B30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="3" t="s">
+      <c r="B32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="3" t="s">
+      <c r="B33" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="B34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="3" t="s">
+      <c r="B35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="3" t="s">
+      <c r="B36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="3" t="s">
+      <c r="B37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="3" t="s">
+      <c r="B38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="3" t="s">
+      <c r="B39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="3" t="s">
+      <c r="B40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>91</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="3" t="s">
+      <c r="B41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E42" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="3" t="s">
+      <c r="B43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F43" s="3" t="s">
+      <c r="E43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="3" t="s">
+      <c r="B44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E44" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="3" t="s">
+      <c r="B45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F45" s="3" t="s">
+      <c r="E45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="3" t="s">
+      <c r="B46" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="3" t="s">
+      <c r="B47" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" s="3" t="s">
+      <c r="B48" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E48" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="3" t="s">
+      <c r="B49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E49" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="3" t="s">
+      <c r="B50" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F50" s="3" t="s">
+      <c r="E50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F50" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="3" t="s">
+      <c r="B51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E51" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="3" t="s">
+      <c r="B52" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E52" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53" s="3" t="s">
+      <c r="B53" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E53" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" s="3" t="s">
+      <c r="B54" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E54" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E55" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56" s="3" t="s">
+      <c r="B56" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E56" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" s="3" t="s">
+      <c r="B57" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="E57" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" s="3" t="s">
+      <c r="B58" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E58" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D59" s="3" t="s">
+      <c r="B59" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="E59" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D60" s="3" t="s">
+      <c r="B60" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E60" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" s="3" t="s">
+      <c r="B62" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="E62" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E63" s="5" t="s">
+      <c r="E63" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="F63" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="3" t="s">
+      <c r="B64" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E64" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65" s="3" t="s">
+      <c r="B65" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="E65" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D66" s="3" t="s">
+      <c r="B66" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="E66" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" s="3" t="s">
+      <c r="B67" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E67" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F67" s="3" t="s">
+      <c r="F67" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" s="3" t="s">
+      <c r="B68" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="E68" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="A69" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D69" s="3" t="s">
+      <c r="B69" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E69" s="4" t="s">
+      <c r="E69" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C70" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="E70" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D71" s="3" t="s">
+      <c r="B71" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="E71" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F71" s="3" t="s">
+      <c r="E71" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D72" s="3" t="s">
+      <c r="B72" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="E72" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="A73" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B73" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D73" s="3" t="s">
+      <c r="B73" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="E73" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="A74" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D74" s="3" t="s">
+      <c r="B74" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E74" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F74" s="3" t="s">
+      <c r="E74" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F74" s="4" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="A75" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D75" s="3" t="s">
+      <c r="B75" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E75" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+      <c r="A76" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D76" s="3" t="s">
+      <c r="B76" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="E76" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="A77" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C77" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="D77" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="E77" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D78" s="3" t="s">
+      <c r="B78" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D78" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E78" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="A79" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D79" s="3" t="s">
+      <c r="B79" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E79" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+      <c r="A80" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" s="3" t="s">
+      <c r="B80" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D80" s="3" t="s">
+      <c r="D80" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="E80" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+      <c r="A81" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B81" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D81" s="3" t="s">
+      <c r="B81" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D81" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="E81" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="A82" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D82" s="3" t="s">
+      <c r="B82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="E82" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F82" s="3" t="s">
+      <c r="E82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F82" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="A83" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B83" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D83" s="3" t="s">
+      <c r="B83" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D83" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E83" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F83" s="3" t="s">
+      <c r="E83" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F83" s="4" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="A84" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D84" s="3" t="s">
+      <c r="B84" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="E84" s="4" t="s">
+      <c r="E84" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="A85" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D85" s="3" t="s">
+      <c r="B85" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="E85" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+      <c r="A86" s="1" t="s">
         <v>191</v>
       </c>
       <c r="B86" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D86" s="3" t="s">
+      <c r="D86" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="E86" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F86" s="3" t="s">
+      <c r="E86" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F86" s="4" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+      <c r="A87" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B87" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D87" s="3" t="s">
+      <c r="B87" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="E87" s="2" t="s">
+      <c r="E87" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+      <c r="A88" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B88" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D88" s="3" t="s">
+      <c r="B88" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D88" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="E88" s="2" t="s">
+      <c r="E88" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+      <c r="A89" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D89" s="3" t="s">
+      <c r="B89" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="E89" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+      <c r="A90" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="3" t="s">
+      <c r="B90" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="D90" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E90" s="2" t="s">
+      <c r="E90" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+      <c r="A91" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D91" s="3" t="s">
+      <c r="B91" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="E91" s="2" t="s">
+      <c r="E91" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
+      <c r="A92" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D92" s="3" t="s">
+      <c r="B92" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="E92" s="5" t="s">
+      <c r="E92" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F92" s="3" t="s">
+      <c r="F92" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
+      <c r="A93" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B93" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D93" s="3" t="s">
+      <c r="B93" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="E93" s="2" t="s">
+      <c r="E93" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
+      <c r="A94" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D94" s="3" t="s">
+      <c r="B94" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="E94" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F94" s="3" t="s">
+      <c r="E94" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F94" s="4" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
+      <c r="A95" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D95" s="3" t="s">
+      <c r="B95" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D95" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="E95" s="2" t="s">
+      <c r="E95" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
+      <c r="A96" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D96" s="3" t="s">
+      <c r="B96" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D96" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="E96" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F96" s="3" t="s">
+      <c r="E96" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F96" s="4" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
+      <c r="A97" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B97" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D97" s="3" t="s">
+      <c r="B97" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D97" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="E97" s="2" t="s">
+      <c r="E97" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
+      <c r="A98" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B98" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D98" s="3" t="s">
+      <c r="B98" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D98" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="E98" s="2" t="s">
+      <c r="E98" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+      <c r="A99" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D99" s="3" t="s">
+      <c r="B99" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D99" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="E99" s="4" t="s">
+      <c r="E99" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
+      <c r="A100" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B100" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B109" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C100" s="3" t="s">
+      <c r="C109" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D100" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="E104" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="E105" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="E107" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="E108" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D109" s="3" t="s">
+      <c r="D109" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="E109" s="2" t="s">
+      <c r="E109" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
+      <c r="A110" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B110" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D110" s="3" t="s">
+      <c r="B110" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D110" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="E110" s="2" t="s">
+      <c r="E110" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
+      <c r="A111" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B111" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D111" s="3" t="s">
+      <c r="B111" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D111" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="E111" s="2" t="s">
+      <c r="E111" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D112" s="0" t="s">
+      <c r="D112" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E112" s="2" t="s">
+      <c r="E112" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D113" s="0" t="s">
+      <c r="D113" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E113" s="4" t="s">
+      <c r="E113" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D114" s="0" t="s">
+      <c r="D114" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E114" s="2" t="s">
+      <c r="E114" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D115" s="0" t="s">
+      <c r="D115" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="E115" s="2" t="s">
+      <c r="E115" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D116" s="0" t="s">
+      <c r="D116" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E116" s="4" t="s">
+      <c r="E116" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D117" s="0" t="s">
+      <c r="D117" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E117" s="2" t="s">
+      <c r="E117" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="1" t="s">
+      <c r="A124" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B124" s="1" t="n">
+      <c r="B124" s="2" t="n">
         <f aca="false">COUNTA(B2:B111)</f>
         <v>110</v>
       </c>
-      <c r="C124" s="1"/>
-      <c r="D124" s="1" t="s">
+      <c r="C124" s="2"/>
+      <c r="D124" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="E124" s="1" t="n">
+      <c r="E124" s="2" t="n">
         <f aca="false">COUNTA(E2:E123)</f>
         <v>116</v>
       </c>
-      <c r="F124" s="1"/>
+      <c r="F124" s="2"/>
     </row>
     <row r="125" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="1" t="s">
+      <c r="A125" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B125" s="1" t="n">
+      <c r="B125" s="2" t="n">
         <f aca="false">COUNTIF(B2:B111, "Playable") + COUNTIF(B2:B109, "Optimized") + COUNTIF(B2:B109, "Remastered")</f>
-        <v>99</v>
-      </c>
-      <c r="C125" s="1"/>
-      <c r="D125" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C125" s="2"/>
+      <c r="D125" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E125" s="1" t="n">
+      <c r="E125" s="2" t="n">
         <f aca="false">COUNTIF(E2:E123, "Playable") + COUNTIF(E2:E123, "Optimized") + COUNTIF(E2:E123, "Remastered")</f>
-        <v>111</v>
-      </c>
-      <c r="F125" s="1"/>
+        <v>112</v>
+      </c>
+      <c r="F125" s="2"/>
     </row>
     <row r="126" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="1" t="s">
+      <c r="A126" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B126" s="1" t="n">
+      <c r="B126" s="2" t="n">
         <f aca="false">ROUND((100/B124)*B125, 1)</f>
-        <v>90</v>
-      </c>
-      <c r="C126" s="1" t="s">
+        <v>90.9</v>
+      </c>
+      <c r="C126" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D126" s="1" t="s">
+      <c r="D126" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="E126" s="1" t="n">
+      <c r="E126" s="2" t="n">
         <f aca="false">ROUND((100/E124)*E125, 1)</f>
-        <v>95.7</v>
-      </c>
-      <c r="F126" s="1" t="s">
+        <v>96.6</v>
+      </c>
+      <c r="F126" s="2" t="s">
         <v>253</v>
       </c>
     </row>

</xml_diff>